<commit_message>
add hostory record for each exercise
</commit_message>
<xml_diff>
--- a/UI2/output/log.xlsx
+++ b/UI2/output/log.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
-  <bookViews>
-    <workbookView activeTab="0"/>
-  </bookViews>
-  <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="exercise 1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="exercise 2" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="exercise 3" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="exercise 4" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="exercise 5" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="exercise 6" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="exercise 7" sheetId="7" state="visible" r:id="rId7"/>
-  </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
-</workbook>
+<s:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <s:workbookPr codeName="ThisWorkbook"/>
+  <s:bookViews>
+    <s:workbookView activeTab="0"/>
+  </s:bookViews>
+  <s:sheets>
+    <s:sheet name="exercise 1" sheetId="1" r:id="rId1"/>
+    <s:sheet name="exercise 2" sheetId="2" r:id="rId2"/>
+    <s:sheet name="exercise 3" sheetId="3" r:id="rId3"/>
+    <s:sheet name="exercise 4" sheetId="4" r:id="rId4"/>
+    <s:sheet name="exercise 5" sheetId="5" r:id="rId5"/>
+    <s:sheet name="exercise 6" sheetId="6" r:id="rId6"/>
+    <s:sheet name="exercise 7" sheetId="7" r:id="rId7"/>
+  </s:sheets>
+  <s:definedNames/>
+  <s:calcPr calcId="124519" fullCalcOnLoad="1"/>
+</s:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="68">
   <si>
     <t>name</t>
   </si>
@@ -46,7 +46,184 @@
     <t>errmsg</t>
   </si>
   <si>
+    <t>Qi Chen</t>
+  </si>
+  <si>
+    <t>male</t>
+  </si>
+  <si>
+    <t>2018-3-15-21-19</t>
+  </si>
+  <si>
     <t>sync_rate</t>
+  </si>
+  <si>
+    <t>2018-3-15-21-20</t>
+  </si>
+  <si>
+    <t>1st right push down lower enough?</t>
+  </si>
+  <si>
+    <t>1st lower right elbow angle</t>
+  </si>
+  <si>
+    <t>1st right hand up straight?</t>
+  </si>
+  <si>
+    <t>1st straight right elbow angle</t>
+  </si>
+  <si>
+    <t>2nd right push down lower enough?</t>
+  </si>
+  <si>
+    <t>2nd lower right elbow angle</t>
+  </si>
+  <si>
+    <t>2nd right hand up straight?</t>
+  </si>
+  <si>
+    <t>2nd straight right elbow angle</t>
+  </si>
+  <si>
+    <t>3rd right push down lower enough?</t>
+  </si>
+  <si>
+    <t>3rd lower right elbow angle</t>
+  </si>
+  <si>
+    <t>3rd right hand up straight?</t>
+  </si>
+  <si>
+    <t>3rd straight right elbow angle</t>
+  </si>
+  <si>
+    <t>4th right push down lower enough?</t>
+  </si>
+  <si>
+    <t>4th lower right elbow angle</t>
+  </si>
+  <si>
+    <t>4th right hand up straight?</t>
+  </si>
+  <si>
+    <t>4th straight right elbow angle</t>
+  </si>
+  <si>
+    <t>average right hand straight angle</t>
+  </si>
+  <si>
+    <t>average right hand push down angle</t>
+  </si>
+  <si>
+    <t>1st left push down lower enough?</t>
+  </si>
+  <si>
+    <t>1st lower left elbow angle</t>
+  </si>
+  <si>
+    <t>1st left hand up straight?</t>
+  </si>
+  <si>
+    <t>1st straight left elbow angle</t>
+  </si>
+  <si>
+    <t>2nd left push down lower enough?</t>
+  </si>
+  <si>
+    <t>2nd lower left elbow angle</t>
+  </si>
+  <si>
+    <t>2nd left hand up straight?</t>
+  </si>
+  <si>
+    <t>2nd straight left elbow angle</t>
+  </si>
+  <si>
+    <t>3rd left push down lower enough?</t>
+  </si>
+  <si>
+    <t>3rd lower left elbow angle</t>
+  </si>
+  <si>
+    <t>3rd left hand up straight?</t>
+  </si>
+  <si>
+    <t>3rd straight left elbow angle</t>
+  </si>
+  <si>
+    <t>4th left push down lower enough?</t>
+  </si>
+  <si>
+    <t>4th lower left elbow angle</t>
+  </si>
+  <si>
+    <t>4th left hand up straight?</t>
+  </si>
+  <si>
+    <t>4th straight left elbow angle</t>
+  </si>
+  <si>
+    <t>average left hand straight angle</t>
+  </si>
+  <si>
+    <t>average left hand push down angle</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Max right bending angle</t>
+  </si>
+  <si>
+    <t>Min right bending angle</t>
+  </si>
+  <si>
+    <t>Max left bending angle</t>
+  </si>
+  <si>
+    <t>Min left bending angle</t>
+  </si>
+  <si>
+    <t>2018-3-15-21-21</t>
+  </si>
+  <si>
+    <t>Max rotation depth</t>
+  </si>
+  <si>
+    <t>Min rotation depth</t>
+  </si>
+  <si>
+    <t>q q</t>
+  </si>
+  <si>
+    <t>2018-3-15-21-53</t>
+  </si>
+  <si>
+    <t>128</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>Max hold time</t>
+  </si>
+  <si>
+    <t>Min hold time</t>
+  </si>
+  <si>
+    <t>average hold time</t>
+  </si>
+  <si>
+    <t>clasp rate</t>
+  </si>
+  <si>
+    <t>2018-3-15-21-25</t>
+  </si>
+  <si>
+    <t>2018-3-15-21-52</t>
   </si>
 </sst>
 </file>
@@ -63,7 +240,11 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="Calibri"/>
+      <family val="2"/>
       <b val="1"/>
+      <color rgb="00000000"/>
+      <sz val="11"/>
     </font>
   </fonts>
   <fills count="2">
@@ -94,14 +275,15 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
@@ -395,13 +577,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
@@ -427,6 +609,29 @@
       </c>
       <c r="H1" s="1" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="n">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="n">
+        <v>43.86390336241045</v>
+      </c>
+      <c r="F2" t="n">
+        <v>77.03703920535486</v>
+      </c>
+      <c r="G2" t="n">
+        <v>57.34908592625425</v>
       </c>
     </row>
   </sheetData>
@@ -440,13 +645,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
@@ -471,10 +676,36 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="n">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="n">
+        <v>46.81015606801768</v>
+      </c>
+      <c r="F2" t="n">
+        <v>70.99227529776917</v>
+      </c>
+      <c r="G2" t="n">
+        <v>59.13905312819104</v>
+      </c>
+      <c r="H2" t="n">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -488,15 +719,15 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:AO2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:41">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -510,7 +741,237 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AO1" s="1" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:41">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="n">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" t="n">
+        <v>47.76393477920845</v>
+      </c>
+      <c r="G2" t="s">
+        <v>49</v>
+      </c>
+      <c r="H2" t="n">
+        <v>163.649948411781</v>
+      </c>
+      <c r="I2" t="s">
+        <v>49</v>
+      </c>
+      <c r="J2" t="n">
+        <v>48.69557300471953</v>
+      </c>
+      <c r="K2" t="s">
+        <v>49</v>
+      </c>
+      <c r="L2" t="n">
+        <v>163.6656187197238</v>
+      </c>
+      <c r="M2" t="s">
+        <v>49</v>
+      </c>
+      <c r="N2" t="n">
+        <v>51.97644221693722</v>
+      </c>
+      <c r="O2" t="s">
+        <v>50</v>
+      </c>
+      <c r="P2" t="n">
+        <v>159.8156410688154</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>49</v>
+      </c>
+      <c r="R2" t="n">
+        <v>49.4745290157706</v>
+      </c>
+      <c r="S2" t="s">
+        <v>49</v>
+      </c>
+      <c r="T2" t="n">
+        <v>166.9884386511605</v>
+      </c>
+      <c r="U2" t="n">
+        <v>163.5299117128702</v>
+      </c>
+      <c r="V2" t="n">
+        <v>49.47761975415895</v>
+      </c>
+      <c r="W2" t="s">
+        <v>49</v>
+      </c>
+      <c r="X2" t="n">
+        <v>40.30816231532291</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>166.6471914449756</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB2" t="n">
+        <v>43.90240944699996</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AD2" t="n">
+        <v>163.6948001072265</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AF2" t="n">
+        <v>41.28694421625423</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AH2" t="n">
+        <v>168.3250424346402</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AJ2" t="n">
+        <v>44.89962183589149</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AL2" t="n">
+        <v>169.7808987903985</v>
+      </c>
+      <c r="AM2" t="n">
+        <v>167.1119831943102</v>
+      </c>
+      <c r="AN2" t="n">
+        <v>42.59928445361714</v>
       </c>
     </row>
   </sheetData>
@@ -530,7 +991,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
@@ -560,15 +1021,15 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -582,7 +1043,45 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="n">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" t="n">
+        <v>61.50235186308937</v>
+      </c>
+      <c r="F2" t="n">
+        <v>53.81505940431422</v>
+      </c>
+      <c r="G2" t="n">
+        <v>61.90373823657983</v>
+      </c>
+      <c r="H2" t="n">
+        <v>44.03911687278126</v>
       </c>
     </row>
   </sheetData>
@@ -596,15 +1095,15 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -618,7 +1117,33 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" t="n">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -632,15 +1157,15 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -654,7 +1179,71 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="n">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E2" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>2.333333333333333</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" t="n">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" t="n">
+        <v>3.533333333333333</v>
+      </c>
+      <c r="F3" t="n">
+        <v>2.066666666666667</v>
+      </c>
+      <c r="G3" t="n">
+        <v>2.673333333333333</v>
+      </c>
+      <c r="H3" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>